<commit_message>
first 6 literature items, appendix
</commit_message>
<xml_diff>
--- a/Diplomarbeit/Literaturverzeichnis.xlsx
+++ b/Diplomarbeit/Literaturverzeichnis.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archive\github\thesis08\Diplomarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062DF6BB-9DF9-4E40-B12E-06A250B97484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4428ED59-93C1-4F72-9121-5FF6B6015E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="180" windowWidth="52215" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="780" windowWidth="52215" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
@@ -28,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="179">
   <si>
     <r>
       <t xml:space="preserve">[1] W. D. Lawson, S. Nielson, E. H. Putley, and A. S. Young. Preparation and properties of HgTe and mixed crystals of </t>
@@ -2443,12 +2452,6 @@
     <t>bibitem</t>
   </si>
   <si>
-    <t>author</t>
-  </si>
-  <si>
-    <t>publication</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -2476,33 +2479,6 @@
     <t>ives</t>
   </si>
   <si>
-    <t>Derek Ives, Nagajara Bezawada.</t>
-  </si>
-  <si>
-    <t>Large area near infra-red detectors for astronomy.</t>
-  </si>
-  <si>
-    <t>W. D. Lawson, S. Nielson, E. H. Putley, and A. S. Young.</t>
-  </si>
-  <si>
-    <t>Preparation and properties of HgTe and mixed crystals of $\mathrm{HgTe}-\mathrm{CdTe}$.</t>
-  </si>
-  <si>
-    <t>J. Phys. Chem. Solids 9, 325-329 (1959).</t>
-  </si>
-  <si>
-    <t>D. Long and J. L. Schmit.</t>
-  </si>
-  <si>
-    <t>Mercury-cadmium telluride and closely related alloys.</t>
-  </si>
-  <si>
-    <t>Gert Finger, J. Garnett, N. Bezawada, R. Dorn, L. Mehrgan, M. Meyer, A. Moorwood, J. Stegmeier, G. Woodhouse.</t>
-  </si>
-  <si>
-    <t>Performance evaluation and calibration issues of large format infrared hybrid active pixel sensors used for ground- and space-based astronomy.</t>
-  </si>
-  <si>
     <t>[40] Yue Wang, Quanbao Li, Qinglin Han, Qinghua Ma, Bingwen Song, Wanqi Jie, Yaohe Zhou, Yuko Inatomi. A two-stage technique for single crystal growth of HgCdTe using a pressurized Bridgman method. Journal of Crystal Growth 263 (2004) 273-282.\\[0pt]</t>
   </si>
   <si>
@@ -2741,6 +2717,81 @@
   </si>
   <si>
     <t>Instruction Manual VUV Discharge Lamp HIS 13.</t>
+  </si>
+  <si>
+    <t>author_and_article</t>
+  </si>
+  <si>
+    <t>publication_italic</t>
+  </si>
+  <si>
+    <t>lawson</t>
+  </si>
+  <si>
+    <t>W. D. Lawson, S. Nielson, E. H. Putley, and A. S. Young. Preparation and properties of HgTe and mixed crystals of $\mathrm{HgTe}-\mathrm{CdTe}$.</t>
+  </si>
+  <si>
+    <t>J. Phys. Chem. Solids</t>
+  </si>
+  <si>
+    <t>{\bfseries 9}, 325-329 (1959).</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>D. Long and J. L. Schmit. Mercury-cadmium telluride and closely related alloys.</t>
+  </si>
+  <si>
+    <t>Semiconductors and Semimetals,</t>
+  </si>
+  <si>
+    <t>Vol. 5, pp. 175-255, edited by R. K. Willardson and A. C. Beer, Academic Press, New York (1970).</t>
+  </si>
+  <si>
+    <t>finger</t>
+  </si>
+  <si>
+    <t>Gert Finger, J. Garnett, N. Bezawada, R. Dorn, L. Mehrgan, M. Meyer, A. Moorwood, J. Stegmeier, G. Woodhouse. Performance evaluation and calibration issues of large format infrared hybrid active pixel sensors used for ground- and space-based astronomy.</t>
+  </si>
+  <si>
+    <t>Nuclear Instruments and Methods in Physics Research</t>
+  </si>
+  <si>
+    <t>{\bfseries A} 565 (2006) 241-250.</t>
+  </si>
+  <si>
+    <t>Derek Ives, Nagajara Bezawada. Large area near infra-red detectors for astronomy.</t>
+  </si>
+  <si>
+    <t>{\bfseries A} 573 (2007) 107-110.</t>
+  </si>
+  <si>
+    <t>gillessen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S. Gillessen, et. al. </t>
+  </si>
+  <si>
+    <t>The Messenger</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 120 (2005) 26-32.</t>
+  </si>
+  <si>
+    <t>groves</t>
+  </si>
+  <si>
+    <t>S. H. Groves, R. N. Brown. C. R. Pidgeon. Interband Magnetoreflection and Band Structure of HgTe.</t>
+  </si>
+  <si>
+    <t>161 (1967), 779.</t>
+  </si>
+  <si>
+    <t>{\bfseries 161} (1967), 779.</t>
+  </si>
+  <si>
+    <t>created-for-LaTeX</t>
   </si>
 </sst>
 </file>
@@ -2825,13 +2876,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3113,845 +3170,1167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="91.28515625" customWidth="1"/>
     <col min="4" max="4" width="112.5703125" customWidth="1"/>
     <col min="5" max="5" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="196.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="101.7109375" customWidth="1"/>
+    <col min="6" max="7" width="101.28515625" customWidth="1"/>
+    <col min="8" max="8" width="101.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>69</v>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="B1" t="s">
         <v>64</v>
       </c>
       <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" t="s">
         <v>66</v>
       </c>
-      <c r="E1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>CONCATENATE("\bibitem{",B2,"} ",C2," {\itshape ",D2,"} ",E2)</f>
+        <v>\bibitem{lawson} W. D. Lawson, S. Nielson, E. H. Putley, and A. S. Young. Preparation and properties of HgTe and mixed crystals of $\mathrm{HgTe}-\mathrm{CdTe}$. {\itshape J. Phys. Chem. Solids} {\bfseries 9}, 325-329 (1959).</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f>CONCATENATE("\bibitem{",B3,"} ",C3," {\itshape ",D3,"} ",E3)</f>
+        <v>\bibitem{long} D. Long and J. L. Schmit. Mercury-cadmium telluride and closely related alloys. {\itshape Semiconductors and Semimetals,} Vol. 5, pp. 175-255, edited by R. K. Willardson and A. C. Beer, Academic Press, New York (1970).</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f>CONCATENATE("\bibitem{",B4,"} ",C4," {\itshape ",D4,"} ",E4)</f>
+        <v>\bibitem{finger} Gert Finger, J. Garnett, N. Bezawada, R. Dorn, L. Mehrgan, M. Meyer, A. Moorwood, J. Stegmeier, G. Woodhouse. Performance evaluation and calibration issues of large format infrared hybrid active pixel sensors used for ground- and space-based astronomy. {\itshape Nuclear Instruments and Methods in Physics Research} {\bfseries A} 565 (2006) 241-250.</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f>CONCATENATE("\bibitem{",B5,"} ",C5," {\itshape ",D5,"} ",E5)</f>
+        <v>\bibitem{ives} Derek Ives, Nagajara Bezawada. Large area near infra-red detectors for astronomy. {\itshape Nuclear Instruments and Methods in Physics Research} {\bfseries A} 573 (2007) 107-110.</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <f>CONCATENATE("\bibitem{",B6,"} ",C6," {\itshape ",D6,"} ",E6)</f>
+        <v>\bibitem{gillessen} S. Gillessen, et. al.  {\itshape The Messenger}  120 (2005) 26-32.</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <f>CONCATENATE("\bibitem{",B7,"} ",C7," {\itshape ",D7,"} ",E7)</f>
+        <v>\bibitem{groves} S. H. Groves, R. N. Brown. C. R. Pidgeon. Interband Magnetoreflection and Band Structure of HgTe. {\itshape 161 (1967), 779.} {\bfseries 161} (1967), 779.</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H45" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H46" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="H47" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H48" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="H49" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H50" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>71</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="H51" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
         <v>63</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="C29" t="s">
-        <v>155</v>
-      </c>
-      <c r="E29" t="s">
-        <v>156</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="C30" t="s">
-        <v>157</v>
-      </c>
-      <c r="D30" t="s">
-        <v>158</v>
-      </c>
-      <c r="E30" t="s">
-        <v>159</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="D31" t="s">
-        <v>164</v>
-      </c>
-      <c r="E31" t="s">
-        <v>160</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>163</v>
-      </c>
-      <c r="D32" t="s">
-        <v>161</v>
-      </c>
-      <c r="E32" t="s">
-        <v>162</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="F46" s="2" t="s">
+      <c r="B64" s="1"/>
+      <c r="C64" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>73</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="C56" t="s">
-        <v>115</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="C63" t="s">
-        <v>105</v>
-      </c>
-      <c r="D63" t="s">
-        <v>106</v>
-      </c>
-      <c r="E63" t="s">
-        <v>107</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="C64" t="s">
-        <v>102</v>
-      </c>
-      <c r="D64" t="s">
-        <v>103</v>
-      </c>
-      <c r="E64" t="s">
-        <v>104</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G64" s="1" t="s">
+      <c r="H64" s="2" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
expand bibliography to original 63 entries
</commit_message>
<xml_diff>
--- a/Diplomarbeit/Literaturverzeichnis.xlsx
+++ b/Diplomarbeit/Literaturverzeichnis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archive\github\thesis08\Diplomarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4428ED59-93C1-4F72-9121-5FF6B6015E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65978D4-3E2A-49A2-A777-9BDC8CB658C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="780" windowWidth="52215" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="30" windowWidth="41805" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="349">
   <si>
     <r>
       <t xml:space="preserve">[1] W. D. Lawson, S. Nielson, E. H. Putley, and A. S. Young. Preparation and properties of HgTe and mixed crystals of </t>
@@ -2530,24 +2530,6 @@
     <t>[63] C. Janowitz, L. Kipp, R. Manzke. Experimental surface band structure of $\mathrm{CdTe}(110)$. Surface Science 231 (1990) 25-31.</t>
   </si>
   <si>
-    <t>C. Janowitz, L. Kipp, R. Manzke.</t>
-  </si>
-  <si>
-    <t>Experimental surface band structure of $\mathrm{CdTe}(110)$.</t>
-  </si>
-  <si>
-    <t>Surface Science 231 (1990) 25-31.</t>
-  </si>
-  <si>
-    <t>E. O. Kane.</t>
-  </si>
-  <si>
-    <t>Band structure of indium antimonide.</t>
-  </si>
-  <si>
-    <t>J. Phys. Chem. Solids 1 (4), 249-261 (1957)</t>
-  </si>
-  <si>
     <t>[62] E. O. Kane. Band structure of indium antimonide. J. Phys. Chem. Solids 1 (4), 249-261 (1957)</t>
   </si>
   <si>
@@ -2569,9 +2551,6 @@
     <t>[55] C. K. Shih, J. A. Silberman, A. K. Wahi, G. P. Carey, I. Lindau, and W. E. Spicer. Angle resolved photoemission study of the alloy scattering effect in $\mathrm{Hg}_{1-\chi} \mathrm{Cd}_{\mathrm{X}}$ Te. J. Vac. Sci. Technol. A, 5(5) pp. 3026-3030 (1987).</t>
   </si>
   <si>
-    <t>C. K. Shih, J. A. Silberman, A. K. Wahi, G. P. Carey, I. Lindau, and W. E. Spicer.</t>
-  </si>
-  <si>
     <t>[1] W. D. Lawson, S. Nielson, E. H. Putley, and A. S. Young. Preparation and properties of HgTe and mixed crystals of $\mathrm{HgTe}-\mathrm{CdTe}$. J. Phys. Chem. Solids 9, 325-329 (1959).</t>
   </si>
   <si>
@@ -2728,9 +2707,6 @@
     <t>lawson</t>
   </si>
   <si>
-    <t>W. D. Lawson, S. Nielson, E. H. Putley, and A. S. Young. Preparation and properties of HgTe and mixed crystals of $\mathrm{HgTe}-\mathrm{CdTe}$.</t>
-  </si>
-  <si>
     <t>J. Phys. Chem. Solids</t>
   </si>
   <si>
@@ -2770,28 +2746,562 @@
     <t>gillessen</t>
   </si>
   <si>
-    <t xml:space="preserve">S. Gillessen, et. al. </t>
-  </si>
-  <si>
     <t>The Messenger</t>
   </si>
   <si>
-    <t xml:space="preserve"> 120 (2005) 26-32.</t>
-  </si>
-  <si>
     <t>groves</t>
   </si>
   <si>
     <t>S. H. Groves, R. N. Brown. C. R. Pidgeon. Interband Magnetoreflection and Band Structure of HgTe.</t>
   </si>
   <si>
-    <t>161 (1967), 779.</t>
-  </si>
-  <si>
     <t>{\bfseries 161} (1967), 779.</t>
   </si>
   <si>
     <t>created-for-LaTeX</t>
+  </si>
+  <si>
+    <t>orlowski</t>
+  </si>
+  <si>
+    <t>Dissertation,</t>
+  </si>
+  <si>
+    <t>AG EES, (2000).</t>
+  </si>
+  <si>
+    <t>higgins</t>
+  </si>
+  <si>
+    <t>ford</t>
+  </si>
+  <si>
+    <t>{\bfseries A} 7 (1989), p 271-275.</t>
+  </si>
+  <si>
+    <t>preuss</t>
+  </si>
+  <si>
+    <t>tanaka</t>
+  </si>
+  <si>
+    <t>W. K. Ford, T. Guo, D. L. Lessor, C. B. Duke. Dynamical low-energy electron-diffraction analysis of bismuth and antimony epitaxy on GaAs(110).</t>
+  </si>
+  <si>
+    <t>H. Hertz. Über den Einfluss des ultravioletten Lichtes auf die elektrische Entladung.</t>
+  </si>
+  <si>
+    <t>Phys. Rev.</t>
+  </si>
+  <si>
+    <t>Ann. Phys.</t>
+  </si>
+  <si>
+    <t>Bertelsmann Universitätsverlag, Düsseldorf, 1974.</t>
+  </si>
+  <si>
+    <t>C. B. Duke. Structure and bonding of tetrahedrally coordinated compound semiconductor cleavage faces.</t>
+  </si>
+  <si>
+    <t>vol. 94 (1989) p. 166-70.</t>
+  </si>
+  <si>
+    <t>gawlik</t>
+  </si>
+  <si>
+    <t>A. Einstein. Über einen die Erzeugung und Verwandlung des Lichtes betreffenden heuristischen Gesichtspunkt.</t>
+  </si>
+  <si>
+    <t>R. Heimburger. Elektronische Eigenschaften und Phasentransformation von $\beta$ - $\mathrm{MoTe}_{2}$.</t>
+  </si>
+  <si>
+    <t>M. Kauert. Vanadiumoxide. Herstellung, Charakterisierung und elektronische Struktur.</t>
+  </si>
+  <si>
+    <t>(1996).</t>
+  </si>
+  <si>
+    <t>seah</t>
+  </si>
+  <si>
+    <t>{\bfseries B} 42, 14 (1990), 8952.</t>
+  </si>
+  <si>
+    <t>duke</t>
+  </si>
+  <si>
+    <t>D. A. Shirley. High-Resolution X-Ray Photoemission Spectrum of the Valence Bands of Gold.</t>
+  </si>
+  <si>
+    <t>A 10(4), 2032 (1992).</t>
+  </si>
+  <si>
+    <t>W. Hallwachs. Über den Einfluss des Lichtes auf elektrostatisch geladene Körper.</t>
+  </si>
+  <si>
+    <t>S. Tougaard. Deconvolution of loss features from electron spectra.</t>
+  </si>
+  <si>
+    <t>{\bfseries 31}, 983 (1887).</t>
+  </si>
+  <si>
+    <t>{\bfseries 33}, 303 (1888).</t>
+  </si>
+  <si>
+    <t>{\bfseries 112}, 117 (1958).</t>
+  </si>
+  <si>
+    <t>einstein</t>
+  </si>
+  <si>
+    <t>tougaard</t>
+  </si>
+  <si>
+    <t>kauert</t>
+  </si>
+  <si>
+    <t>{\bfseries 17} (1905), 132-148.</t>
+  </si>
+  <si>
+    <t>AG EES, (2007).</t>
+  </si>
+  <si>
+    <t>huefner</t>
+  </si>
+  <si>
+    <t>Platin-Widerstandsthermometer Pt100 nach IEC 751 / DIN EN 60751.</t>
+  </si>
+  <si>
+    <t>Springer-Verlag Berlin Heidelberg New York 2003.</t>
+  </si>
+  <si>
+    <t>T. Plake. Aufbau und Inbetriebnahme des Photoemissionsexperimentes HIRE-PES: Charakterisierung und erste Untersuchungen an $\mathrm{Bi}_{2} \mathrm{Sr}_{2} \mathrm{CuO}_{6}$-Hochtemperatursupraleitern.</t>
+  </si>
+  <si>
+    <t>C. Janowitz, R. Müller, T. Plake, Th. Böger, R. Manzke. New high-resolution photoemission station for synchrotron radiation at BESSY.</t>
+  </si>
+  <si>
+    <t>Diplomarbeit,</t>
+  </si>
+  <si>
+    <t>Softwarepaket: Origin 7.5 SR5, \href{http://www.OriginLab.com}{http://www.OriginLab.com} (2004)</t>
+  </si>
+  <si>
+    <t>A. Savitzky, Marcel J.E. Golay. Smoothing and Differentiation of Data by Simplified Least Squares Procedures.</t>
+  </si>
+  <si>
+    <t>Analytical Chemistry,</t>
+  </si>
+  <si>
+    <t>Vol. 1, Issue 1, p 2-11 (1979).</t>
+  </si>
+  <si>
+    <t>{\bfseries B} 5, 4709-4714 (1972).</t>
+  </si>
+  <si>
+    <t>139 (1984) pp. 208-218.</t>
+  </si>
+  <si>
+    <t>savitzky</t>
+  </si>
+  <si>
+    <t>36: 1627-1639 (1964). doi:10.1021/ac60214a047</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>plake</t>
+  </si>
+  <si>
+    <t>AG EES, (1998).</t>
+  </si>
+  <si>
+    <t>janowitz</t>
+  </si>
+  <si>
+    <t>M. Martins, G. Kaindl, N. Schwentner. Design of the high-resolution BUS XUV-beamline for BESSY II.</t>
+  </si>
+  <si>
+    <t>Journal of Electron Spectroscopy and Related Phenomena</t>
+  </si>
+  <si>
+    <t>105, 43-49 (1999).</t>
+  </si>
+  <si>
+    <t>purcell</t>
+  </si>
+  <si>
+    <t>mante</t>
+  </si>
+  <si>
+    <t>omicron</t>
+  </si>
+  <si>
+    <t>pt100</t>
+  </si>
+  <si>
+    <t>martins</t>
+  </si>
+  <si>
+    <t>colombo</t>
+  </si>
+  <si>
+    <t>wang</t>
+  </si>
+  <si>
+    <t>orlowski2</t>
+  </si>
+  <si>
+    <t>brice</t>
+  </si>
+  <si>
+    <t>P. Norton. HgCdTe infrared detectors.</t>
+  </si>
+  <si>
+    <t>Yue Wang, Quanbao Li, Qinglin Han, Qinghua Ma, Bingwen Song, Wanqi Jie, Yaohe Zhou, Yuko Inatomi. A two-stage technique for single crystal growth of HgCdTe using a pressurized Bridgman method.</t>
+  </si>
+  <si>
+    <t>Opto-Electronics Review</t>
+  </si>
+  <si>
+    <t>101-103, 965-969 (1999).</t>
+  </si>
+  <si>
+    <t>J. C. Brice. Properties of Mercury Cadmium Telluride.</t>
+  </si>
+  <si>
+    <t>61, R5058-R5061, (2000).</t>
+  </si>
+  <si>
+    <t>No 3. INSPEC, IEE, p. 3 (1994).</t>
+  </si>
+  <si>
+    <t>hansen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {\bfseries 53}, 7099-7101 (1982).</t>
+  </si>
+  <si>
+    <t>norton</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {\bfseries 10}(3), 159-174 (2002).</t>
+  </si>
+  <si>
+    <t>vere</t>
+  </si>
+  <si>
+    <t>vol. 59 (1982) p. 121-129.</t>
+  </si>
+  <si>
+    <t>A 3(1), 100-104 (1985).</t>
+  </si>
+  <si>
+    <t>263 (2004) 273-282.</t>
+  </si>
+  <si>
+    <t>colombo2</t>
+  </si>
+  <si>
+    <t>A 6(4), 2795-2799 (1988).</t>
+  </si>
+  <si>
+    <t>harman</t>
+  </si>
+  <si>
+    <t>T. C. Harman. Optically pumped LPE-grown $\mathrm{Hg}_{1-\mathrm{x}} \mathrm{Cd}_{\mathrm{X}} \mathrm{Te}$ lasers.</t>
+  </si>
+  <si>
+    <t>vol. 8 (1979) p. 191-200.</t>
+  </si>
+  <si>
+    <t>koo</t>
+  </si>
+  <si>
+    <t>B66, 7074, (1999).</t>
+  </si>
+  <si>
+    <t>wang2</t>
+  </si>
+  <si>
+    <t>263 (2004) 54-62.</t>
+  </si>
+  <si>
+    <t>nikiforov</t>
+  </si>
+  <si>
+    <t>capper</t>
+  </si>
+  <si>
+    <t>Properties of narrow gap Cadmium-based compounds.</t>
+  </si>
+  <si>
+    <t>INSPEC, the Institution of Electrical Engineers (1994).</t>
+  </si>
+  <si>
+    <t>williams</t>
+  </si>
+  <si>
+    <t>vol. 83 (1987) p. 341-352.</t>
+  </si>
+  <si>
+    <t>1(3) pp. 1735-1743 (1983).</t>
+  </si>
+  <si>
+    <t>morgen</t>
+  </si>
+  <si>
+    <t>56, 493-497 (1982).</t>
+  </si>
+  <si>
+    <t>mitdank</t>
+  </si>
+  <si>
+    <t>berding</t>
+  </si>
+  <si>
+    <t>vol.  {\bfseries 5} pp. S86-S89 (1990).</t>
+  </si>
+  <si>
+    <t>ribbat</t>
+  </si>
+  <si>
+    <t>silberman</t>
+  </si>
+  <si>
+    <t>21(1) pp. 142-145 (1982).</t>
+  </si>
+  <si>
+    <t>shih</t>
+  </si>
+  <si>
+    <t>5(5) pp. 3031-3034 (1987).</t>
+  </si>
+  <si>
+    <t>shih2</t>
+  </si>
+  <si>
+    <t>5(5) pp. 3026-3030 (1987).</t>
+  </si>
+  <si>
+    <t>puettner</t>
+  </si>
+  <si>
+    <t>Dr. Ralph Püttner, FU Berlin. Beamlinebetreuer BUS. Private communication.</t>
+  </si>
+  <si>
+    <t>moon</t>
+  </si>
+  <si>
+    <t>{\bfseries B} 74:045205 (2006).</t>
+  </si>
+  <si>
+    <t>moulder</t>
+  </si>
+  <si>
+    <t>Perkin-Elmer Corporation, 1992.</t>
+  </si>
+  <si>
+    <t>janowitz2</t>
+  </si>
+  <si>
+    <t>328, 84-89, (2001).</t>
+  </si>
+  <si>
+    <t>fleszar</t>
+  </si>
+  <si>
+    <t>{\bfseries B} 71:045207 (2005).</t>
+  </si>
+  <si>
+    <t>chen</t>
+  </si>
+  <si>
+    <t>kane</t>
+  </si>
+  <si>
+    <t>janowitz3</t>
+  </si>
+  <si>
+    <t>1 (4), 249-261 (1957)</t>
+  </si>
+  <si>
+    <t>231 (1990) 25-31.</t>
+  </si>
+  <si>
+    <t>120 (2005) 26-32.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vakuum Science and Technology</t>
+  </si>
+  <si>
+    <t>Laue Atlas. Plotted Laue Back-Reflection Patterns of the Elements, the Compounds $R X$ and $R X_{2}$.</t>
+  </si>
+  <si>
+    <t>J. Cryst. Growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> J. Vac. Sci. Technol.</t>
+  </si>
+  <si>
+    <t>S. Gillessen, et. al.</t>
+  </si>
+  <si>
+    <t>N. Orlowski. Untersuchung der elektronischen Struktur von HgSe und HgTe mittels winkelaufgelöster Photoemission.</t>
+  </si>
+  <si>
+    <t>E. Preuss, B. Krahn-Urban, R. Butz.</t>
+  </si>
+  <si>
+    <t>A. Tanaka, Y. Masa, S. Seto, T. Kawasaki. Zinc and selenium co-doped CdTe substrates lattice matched to HgCdTe.</t>
+  </si>
+  <si>
+    <t>W. E. Spicer. Photoemissive, Photoconductive, and Optical Absorption Studies of AlkaliAntimony Compounds</t>
+  </si>
+  <si>
+    <t>Stefan Hüfner.</t>
+  </si>
+  <si>
+    <t>M. P. Seah, W. A. Dench. Quantitative Electron Spectroscopy of Surface: A Standard Data Base for Electron Inelastic Mean Free Paths in Solids.</t>
+  </si>
+  <si>
+    <t>N. Orlowski, J. Augustin, Z. Golacki, C. Janowitz, R. Manzke. Direct evidence for the inverted band structure of HgTe.</t>
+  </si>
+  <si>
+    <t>L. Colombo, A. J. Syllaios, r. W. Perlaky, M. J. Brau. Growth of large diameter (Hg,Cd)Te crystals by incremental quenching.</t>
+  </si>
+  <si>
+    <t>L. Colombo, R. R. Chang, C. J. Chang, B. A. Baird. Growth of Hg-based alloys by the traveling heater method.</t>
+  </si>
+  <si>
+    <t>B. H. Koo, Y. Ishikawa, J.F. Wang, M. Isshiki. Crowth of $\mathrm{Hg}_{1-\mathrm{x}}\left(\mathrm{Cd}_{1-\mathrm{y}} \mathrm{Zn}_{\mathrm{y}}\right)_{\mathrm{x}} \mathrm{Te}$ epilayers on (100) $\mathrm{Cd}_{1-\mathrm{y}} \mathrm{Zn}_{\mathrm{y}} \mathrm{Te} / \mathrm{GaAs}$ substrates by ISOVPE.</t>
+  </si>
+  <si>
+    <t>Yue Wang, Quanbao Li, Qinglin Han, Qinghua Ma, Rongbin Ji, Bingwen Song, Wanqi Jie, Yaohe Zhou, Yuko Inatomi. Growth and properties of 40 mm diameter $\mathrm{Hg}_{1-\chi} \mathrm{Cd}_{\mathrm{X}} \mathrm{Te}$ using the two-stage Pressurized Bridgman method.</t>
+  </si>
+  <si>
+    <t>Vladimir Nikiforov (\ru{Никифоров Владимир Николаевиш}), MSU, Private communication.</t>
+  </si>
+  <si>
+    <t>P. Capper.</t>
+  </si>
+  <si>
+    <t>D. J. Williams, A. W. Vere. Sub-grain boundaries in $\mathrm{Cd}_{\mathrm{X}} \mathrm{Hg}_{1-\mathrm{X}} \mathrm{Te}$ and CdTe.</t>
+  </si>
+  <si>
+    <t>W. E. Spicer, J. A. Silberman, and I. Lindau. Band gap variation and lattice, surface, and interface "instabilities" in $\mathrm{Hg}_{1-\mathrm{x}} \mathrm{Cd}_{\mathrm{x}} \mathrm{Te}$ and related compounds.</t>
+  </si>
+  <si>
+    <t>E. O. Kane. Band structure of indium antimonide.</t>
+  </si>
+  <si>
+    <t>A-B Chen, Y-M Lai-Hsu, S. Krishnamurthy, M. A. Berding, and A. Sher. Band structures of HgCdTe and HgZnTe alloys and superlattices.</t>
+  </si>
+  <si>
+    <t>A. Fleszar, W. Hanke. Electronic structure of $\mathrm{II}^{\mathrm{B}}$-VI semiconductors in the GW approximation.</t>
+  </si>
+  <si>
+    <t>C. Janowitz, N. Orlowski, R. Manzke, Z. Golacki. On the band structure of HgTe and HgSe - view from photoemission.</t>
+  </si>
+  <si>
+    <t>J. F. Moulder, W. F. Stickle, P. E. Sobol, K. D. Bomben.</t>
+  </si>
+  <si>
+    <t>C. K. Shih and W. E. Spicer. Photoemission studies of core level shifts in $\mathrm{HgCdTe}, \mathrm{CdMnTe}$, and HgZnTe.</t>
+  </si>
+  <si>
+    <t>C. Ribbat. Aufbau einer MBE-Anlage zur Herstellung von MolybdändichalkogenidSchichtkristallen für photovoltaische Anwendungen.</t>
+  </si>
+  <si>
+    <t>M. A. Berding, A. Sher, A-B Chen and R. Patrick. Vacancies and surface segregation in HgCdTe and HgZnTe.</t>
+  </si>
+  <si>
+    <t>P. Morgen, J. Silberman, I. Landau, W. E. Spicer, J. A. Wilson. Stability of an atomically clean $\mathrm{Hg}_{1-\mathrm{x}} \mathrm{Cd}_{\mathrm{x}} \mathrm{Te}$ surface in vacuum and under $\mathrm{O}_{2}$ exposure.</t>
+  </si>
+  <si>
+    <t>Surface Science</t>
+  </si>
+  <si>
+    <t>Semicond. Sci. Technol.</t>
+  </si>
+  <si>
+    <t>Journal of Alloys and Compounds,</t>
+  </si>
+  <si>
+    <t>Handbook of X-ray Photoelectron Spectroscopy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> J. Vac. Sci. Technol. A,</t>
+  </si>
+  <si>
+    <t>J. Vac. Sci. Technol. A,</t>
+  </si>
+  <si>
+    <t>J. Vac. Sci. Technol.</t>
+  </si>
+  <si>
+    <t>Journal of Crystal Growth</t>
+  </si>
+  <si>
+    <t>J. Vac. Sci. Technol. A</t>
+  </si>
+  <si>
+    <t>Materials Science and Engineering,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> J. Electron. Mater.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> J. Appl. Phys.</t>
+  </si>
+  <si>
+    <t>EMIS Datareviews Series</t>
+  </si>
+  <si>
+    <t>Phys. Rev. B, Rapid Communications,</t>
+  </si>
+  <si>
+    <t>Surface and Interface Analysis,</t>
+  </si>
+  <si>
+    <t>Photoelectron Spectroscopy, Principles and Applications, Third Edition.</t>
+  </si>
+  <si>
+    <t>Annalen der Physik</t>
+  </si>
+  <si>
+    <t>Chang-Youn Moon, Su-Huai Wei. Band gap of Hg chalcogenides: Symmetry-reduction-induced band-gap opening of materials with inverted band structures.</t>
+  </si>
+  <si>
+    <t>W. D. Lawson, S. Nielson, E. H. Putley, and A. S. Young. Preparation and properties of HgTe and mixed crystals of HgTe-CdTe.</t>
+  </si>
+  <si>
+    <t>K.-U. Gawlik. Untersuchung der elektronischen Struktur von II-VI-Verbindungshalb-leitern mit direkter und inverser Photoemission.</t>
+  </si>
+  <si>
+    <t>R. Mitdank. Mikrosondenanalyse. Beispiele für Untersuchungen an der Elektronenstrahlmikrosonde. \href{http://htc.physik.hu-berlin.de/~mitdank/semq.htm}{http://htc.physik.hu-berlin.de/~mitdank/semq.htm}.</t>
+  </si>
+  <si>
+    <t>vol. {\bfseries 5} pp. S100-S102 (1990). doi:\href{http://dx.doi.org/10.1088/0268-1242/5/3S/021}{10.1088/0268-1242/5/3S/021}</t>
+  </si>
+  <si>
+    <t>C. Janowitz, L. Kipp, R. Manzke. Experimental surface band structure of CdTe(110).</t>
+  </si>
+  <si>
+    <t>J. A. Silberman, P. Morgen, I. Lindau, and W. E. Spicer. UPS study of the electronic structure of $\mathrm{Hg_{1-X}Cd_XTe}$: Breakdown of the virtual crystal approximation.</t>
+  </si>
+  <si>
+    <t>C. K. Shih, J. A. Silberman, A. K. Wahi, G. P. Carey, I. Lindau, and W. E. Spicer. Angle resolved photoemission study of the alloy scattering effect in $\mathrm{Hg_{1-X}Cd_XTe}$.</t>
+  </si>
+  <si>
+    <t>G. L. Hansen, J. L. Schmit, and T. N. Casselman. Energy gap versus alloy composition and temperature in Hg\textsubscript{1-X}Cd\textsubscript{X}Te</t>
+  </si>
+  <si>
+    <t>A. W. Vere, B. W. Straughan, D. J. Williams, N. Shaw, A. Royle, J. S. Gough, J. B. Mullin. Growth of Cd\textsubscript{X}Hg\textsubscript{1-X}Te by a pressurised cast-recrystallise-anneal technique,</t>
+  </si>
+  <si>
+    <t>W. M. Higgins, G. N. Pultz, R. G. Roy, R. A. Lancaster, J. L. Schmit. Standard relationships in the properties of Hg\textsubscript{1-x}Cd\textsubscript{x}Te.</t>
   </si>
 </sst>
 </file>
@@ -2892,7 +3402,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3173,18 +3683,19 @@
   <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="91.28515625" customWidth="1"/>
-    <col min="4" max="4" width="112.5703125" customWidth="1"/>
-    <col min="5" max="5" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="101.28515625" customWidth="1"/>
+    <col min="3" max="3" width="69.42578125" customWidth="1"/>
+    <col min="4" max="4" width="56.85546875" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
+    <col min="6" max="6" width="90.85546875" customWidth="1"/>
+    <col min="7" max="7" width="101.28515625" customWidth="1"/>
     <col min="8" max="8" width="101.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3196,16 +3707,16 @@
         <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E1" t="s">
         <v>65</v>
       </c>
       <c r="F1" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="G1" t="s">
         <v>66</v>
@@ -3219,23 +3730,23 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>157</v>
+        <v>339</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f>CONCATENATE("\bibitem{",B2,"} ",C2," {\itshape ",D2,"} ",E2)</f>
-        <v>\bibitem{lawson} W. D. Lawson, S. Nielson, E. H. Putley, and A. S. Young. Preparation and properties of HgTe and mixed crystals of $\mathrm{HgTe}-\mathrm{CdTe}$. {\itshape J. Phys. Chem. Solids} {\bfseries 9}, 325-329 (1959).</v>
+        <f t="shared" ref="F2:F64" si="0">CONCATENATE("\bibitem{",B2,"} ",C2," {\itshape ",D2,"} ",E2)</f>
+        <v>\bibitem{lawson} W. D. Lawson, S. Nielson, E. H. Putley, and A. S. Young. Preparation and properties of HgTe and mixed crystals of HgTe-CdTe. {\itshape J. Phys. Chem. Solids} {\bfseries 9}, 325-329 (1959).</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>0</v>
@@ -3246,23 +3757,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f>CONCATENATE("\bibitem{",B3,"} ",C3," {\itshape ",D3,"} ",E3)</f>
+        <f t="shared" si="0"/>
         <v>\bibitem{long} D. Long and J. L. Schmit. Mercury-cadmium telluride and closely related alloys. {\itshape Semiconductors and Semimetals,} Vol. 5, pp. 175-255, edited by R. K. Willardson and A. C. Beer, Academic Press, New York (1970).</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>1</v>
@@ -3273,29 +3784,29 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>CONCATENATE("\bibitem{",B4,"} ",C4," {\itshape ",D4,"} ",E4)</f>
+        <f t="shared" si="0"/>
         <v>\bibitem{finger} Gert Finger, J. Garnett, N. Bezawada, R. Dorn, L. Mehrgan, M. Meyer, A. Moorwood, J. Stegmeier, G. Woodhouse. Performance evaluation and calibration issues of large format infrared hybrid active pixel sensors used for ground- and space-based astronomy. {\itshape Nuclear Instruments and Methods in Physics Research} {\bfseries A} 565 (2006) 241-250.</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3303,74 +3814,74 @@
         <v>73</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f>CONCATENATE("\bibitem{",B5,"} ",C5," {\itshape ",D5,"} ",E5)</f>
+        <f t="shared" si="0"/>
         <v>\bibitem{ives} Derek Ives, Nagajara Bezawada. Large area near infra-red detectors for astronomy. {\itshape Nuclear Instruments and Methods in Physics Research} {\bfseries A} 573 (2007) 107-110.</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>171</v>
+        <v>296</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>173</v>
+        <v>291</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f>CONCATENATE("\bibitem{",B6,"} ",C6," {\itshape ",D6,"} ",E6)</f>
-        <v>\bibitem{gillessen} S. Gillessen, et. al.  {\itshape The Messenger}  120 (2005) 26-32.</v>
+        <f t="shared" si="0"/>
+        <v>\bibitem{gillessen} S. Gillessen, et. al. {\itshape The Messenger} 120 (2005) 26-32.</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f>CONCATENATE("\bibitem{",B7,"} ",C7," {\itshape ",D7,"} ",E7)</f>
-        <v>\bibitem{groves} S. H. Groves, R. N. Brown. C. R. Pidgeon. Interband Magnetoreflection and Band Structure of HgTe. {\itshape 161 (1967), 779.} {\bfseries 161} (1967), 779.</v>
+        <f t="shared" si="0"/>
+        <v>\bibitem{groves} S. H. Groves, R. N. Brown. C. R. Pidgeon. Interband Magnetoreflection and Band Structure of HgTe. {\itshape Phys. Rev.} {\bfseries 161} (1967), 779.</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>5</v>
@@ -3380,13 +3891,24 @@
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{orlowski} N. Orlowski. Untersuchung der elektronischen Struktur von HgSe und HgTe mittels winkelaufgelöster Photoemission. {\itshape Diplomarbeit,} AG EES, (2000).</v>
+      </c>
       <c r="G8" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>6</v>
@@ -3396,29 +3918,51 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{higgins} W. M. Higgins, G. N. Pultz, R. G. Roy, R. A. Lancaster, J. L. Schmit. Standard relationships in the properties of Hg\textsubscript{1-x}Cd\textsubscript{x}Te. {\itshape  Vakuum Science and Technology} {\bfseries A} 7 (1989), p 271-275.</v>
+      </c>
       <c r="G9" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{preuss} E. Preuss, B. Krahn-Urban, R. Butz. {\itshape Laue Atlas. Plotted Laue Back-Reflection Patterns of the Elements, the Compounds $R X$ and $R X_{2}$.} Bertelsmann Universitätsverlag, Düsseldorf, 1974.</v>
+      </c>
       <c r="G10" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>8</v>
@@ -3428,13 +3972,24 @@
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{tanaka} A. Tanaka, Y. Masa, S. Seto, T. Kawasaki. Zinc and selenium co-doped CdTe substrates lattice matched to HgCdTe. {\itshape J. Cryst. Growth} vol. 94 (1989) p. 166-70.</v>
+      </c>
       <c r="G11" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>9</v>
@@ -3444,29 +3999,51 @@
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{gawlik} K.-U. Gawlik. Untersuchung der elektronischen Struktur von II-VI-Verbindungshalb-leitern mit direkter und inverser Photoemission. {\itshape Dissertation,} (1996).</v>
+      </c>
       <c r="G12" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{ford} W. K. Ford, T. Guo, D. L. Lessor, C. B. Duke. Dynamical low-energy electron-diffraction analysis of bismuth and antimony epitaxy on GaAs(110). {\itshape Phys. Rev.} {\bfseries B} 42, 14 (1990), 8952.</v>
+      </c>
       <c r="G13" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>11</v>
@@ -3476,13 +4053,24 @@
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{duke} C. B. Duke. Structure and bonding of tetrahedrally coordinated compound semiconductor cleavage faces. {\itshape  J. Vac. Sci. Technol.} A 10(4), 2032 (1992).</v>
+      </c>
       <c r="G14" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>12</v>
@@ -3495,46 +4083,75 @@
       <c r="B15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{hertz} H. Hertz. Über den Einfluss des ultravioletten Lichtes auf die elektrische Entladung. {\itshape Ann. Phys.} {\bfseries 31}, 983 (1887).</v>
+      </c>
       <c r="G15" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{hallwachs} W. Hallwachs. Über den Einfluss des Lichtes auf elektrostatisch geladene Körper. {\itshape Ann. Phys.} {\bfseries 33}, 303 (1888).</v>
+      </c>
       <c r="G16" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F17" s="1" t="str">
+        <f>CONCATENATE("\bibitem{",B17,"} ",C17," {\itshape ",D17,"} ",E17)</f>
+        <v>\bibitem{einstein} A. Einstein. Über einen die Erzeugung und Verwandlung des Lichtes betreffenden heuristischen Gesichtspunkt. {\itshape Annalen der Physik} {\bfseries 17} (1905), 132-148.</v>
+      </c>
       <c r="G17" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>15</v>
@@ -3547,12 +4164,21 @@
       <c r="B18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{spicer1} W. E. Spicer. Photoemissive, Photoconductive, and Optical Absorption Studies of AlkaliAntimony Compounds {\itshape Phys. Rev.} {\bfseries 112}, 117 (1958).</v>
+      </c>
       <c r="G18" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>16</v>
@@ -3562,13 +4188,24 @@
       <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{huefner} Stefan Hüfner. {\itshape Photoelectron Spectroscopy, Principles and Applications, Third Edition.} Springer-Verlag Berlin Heidelberg New York 2003.</v>
+      </c>
       <c r="G19" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>17</v>
@@ -3581,28 +4218,48 @@
       <c r="B20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{heimburger} R. Heimburger. Elektronische Eigenschaften und Phasentransformation von $\beta$ - $\mathrm{MoTe}_{2}$. {\itshape Diplomarbeit,} AG EES, (2007).</v>
+      </c>
       <c r="G20" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{seah} M. P. Seah, W. A. Dench. Quantitative Electron Spectroscopy of Surface: A Standard Data Base for Electron Inelastic Mean Free Paths in Solids. {\itshape Surface and Interface Analysis,} Vol. 1, Issue 1, p 2-11 (1979).</v>
+      </c>
       <c r="G21" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>19</v>
@@ -3615,28 +4272,48 @@
       <c r="B22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{shirley} D. A. Shirley. High-Resolution X-Ray Photoemission Spectrum of the Valence Bands of Gold. {\itshape Phys. Rev.} {\bfseries B} 5, 4709-4714 (1972).</v>
+      </c>
       <c r="G22" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{tougaard} S. Tougaard. Deconvolution of loss features from electron spectra. {\itshape Surface Science} 139 (1984) pp. 208-218.</v>
+      </c>
       <c r="G23" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>21</v>
@@ -3646,77 +4323,128 @@
       <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{kauert} M. Kauert. Vanadiumoxide. Herstellung, Charakterisierung und elektronische Struktur. {\itshape Diplomarbeit,} AG EES, (2007).</v>
+      </c>
       <c r="G24" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{savitzky} A. Savitzky, Marcel J.E. Golay. Smoothing and Differentiation of Data by Simplified Least Squares Procedures. {\itshape Analytical Chemistry,} 36: 1627-1639 (1964). doi:10.1021/ac60214a047</v>
+      </c>
       <c r="G25" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="F26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">\bibitem{origin} Softwarepaket: Origin 7.5 SR5, \href{http://www.OriginLab.com}{http://www.OriginLab.com} (2004) {\itshape } </v>
+      </c>
       <c r="G26" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{plake} T. Plake. Aufbau und Inbetriebnahme des Photoemissionsexperimentes HIRE-PES: Charakterisierung und erste Untersuchungen an $\mathrm{Bi}_{2} \mathrm{Sr}_{2} \mathrm{CuO}_{6}$-Hochtemperatursupraleitern. {\itshape Diplomarbeit,} AG EES, (1998).</v>
+      </c>
       <c r="G27" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{janowitz} C. Janowitz, R. Müller, T. Plake, Th. Böger, R. Manzke. New high-resolution photoemission station for synchrotron radiation at BESSY. {\itshape Journal of Electron Spectroscopy and Related Phenomena} 105, 43-49 (1999).</v>
+      </c>
       <c r="G28" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>26</v>
@@ -3726,17 +4454,22 @@
       <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="C29" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F29" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="F29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{purcell} E. Purcell. {\itshape } Phys. Rev. 54 (1938) 818.</v>
+      </c>
       <c r="G29" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>27</v>
@@ -3746,109 +4479,151 @@
       <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="C30" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F30" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="F30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{mante} G. Mante. {\itshape Doktorarbeit,} Universität Kiel (1992).</v>
+      </c>
       <c r="G30" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F31" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="F31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{omicron}  {\itshape Instruction Manual VUV Discharge Lamp HIS 13.} Omicron Vakuumphysik GmbH (\href{http://www.omicron.de}{www.omicron.de}).</v>
+      </c>
       <c r="G31" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F32" s="1"/>
+        <v>227</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">\bibitem{pt100} Platin-Widerstandsthermometer Pt100 nach IEC 751 / DIN EN 60751. {\itshape } </v>
+      </c>
       <c r="G32" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{ar65view}  {\itshape AR65view.} Java-Software zur Analyse und Manipulation der Messdaten von AR65 und WESPHOA. \href{http://sourceforge.net/projects/ar65view/}{sourceforge.net/projects/ar65view/}.</v>
+      </c>
       <c r="G33" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{martins} M. Martins, G. Kaindl, N. Schwentner. Design of the high-resolution BUS XUV-beamline for BESSY II. {\itshape Journal of Electron Spectroscopy and Related Phenomena} 101-103, 965-969 (1999).</v>
+      </c>
       <c r="G34" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{orlowski2} N. Orlowski, J. Augustin, Z. Golacki, C. Janowitz, R. Manzke. Direct evidence for the inverted band structure of HgTe. {\itshape Phys. Rev. B, Rapid Communications,} 61, R5058-R5061, (2000).</v>
+      </c>
       <c r="G35" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>33</v>
@@ -3858,61 +4633,105 @@
       <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{brice} J. C. Brice. Properties of Mercury Cadmium Telluride. {\itshape EMIS Datareviews Series} No 3. INSPEC, IEE, p. 3 (1994).</v>
+      </c>
       <c r="G36" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{hansen} G. L. Hansen, J. L. Schmit, and T. N. Casselman. Energy gap versus alloy composition and temperature in Hg\textsubscript{1-X}Cd\textsubscript{X}Te {\itshape  J. Appl. Phys.}  {\bfseries 53}, 7099-7101 (1982).</v>
+      </c>
       <c r="G37" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{norton} P. Norton. HgCdTe infrared detectors. {\itshape Opto-Electronics Review}  {\bfseries 10}(3), 159-174 (2002).</v>
+      </c>
       <c r="G38" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{vere} A. W. Vere, B. W. Straughan, D. J. Williams, N. Shaw, A. Royle, J. S. Gough, J. B. Mullin. Growth of Cd\textsubscript{X}Hg\textsubscript{1-X}Te by a pressurised cast-recrystallise-anneal technique, {\itshape J. Cryst. Growth} vol. 59 (1982) p. 121-129.</v>
+      </c>
       <c r="G39" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>37</v>
@@ -3922,13 +4741,24 @@
       <c r="A40" s="4">
         <v>39</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{colombo} L. Colombo, A. J. Syllaios, r. W. Perlaky, M. J. Brau. Growth of large diameter (Hg,Cd)Te crystals by incremental quenching. {\itshape J. Vac. Sci. Technol.} A 3(1), 100-104 (1985).</v>
+      </c>
       <c r="G40" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>38</v>
@@ -3938,11 +4768,22 @@
       <c r="A41" s="4">
         <v>40</v>
       </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{wang} Yue Wang, Quanbao Li, Qinglin Han, Qinghua Ma, Bingwen Song, Wanqi Jie, Yaohe Zhou, Yuko Inatomi. A two-stage technique for single crystal growth of HgCdTe using a pressurized Bridgman method. {\itshape Journal of Crystal Growth} 263 (2004) 273-282.</v>
+      </c>
       <c r="G41" s="1" t="s">
         <v>74</v>
       </c>
@@ -3954,11 +4795,22 @@
       <c r="A42" s="4">
         <v>41</v>
       </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{colombo2} L. Colombo, R. R. Chang, C. J. Chang, B. A. Baird. Growth of Hg-based alloys by the traveling heater method. {\itshape J. Vac. Sci. Technol.} A 6(4), 2795-2799 (1988).</v>
+      </c>
       <c r="G42" s="1" t="s">
         <v>75</v>
       </c>
@@ -3966,15 +4818,26 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>42</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{harman} T. C. Harman. Optically pumped LPE-grown $\mathrm{Hg}_{1-\mathrm{x}} \mathrm{Cd}_{\mathrm{X}} \mathrm{Te}$ lasers. {\itshape  J. Electron. Mater.} vol. 8 (1979) p. 191-200.</v>
+      </c>
       <c r="G43" s="1" t="s">
         <v>76</v>
       </c>
@@ -3982,15 +4845,26 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
+      <c r="B44" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{koo} B. H. Koo, Y. Ishikawa, J.F. Wang, M. Isshiki. Crowth of $\mathrm{Hg}_{1-\mathrm{x}}\left(\mathrm{Cd}_{1-\mathrm{y}} \mathrm{Zn}_{\mathrm{y}}\right)_{\mathrm{x}} \mathrm{Te}$ epilayers on (100) $\mathrm{Cd}_{1-\mathrm{y}} \mathrm{Zn}_{\mathrm{y}} \mathrm{Te} / \mathrm{GaAs}$ substrates by ISOVPE. {\itshape Materials Science and Engineering,} B66, 7074, (1999).</v>
+      </c>
       <c r="G44" s="1" t="s">
         <v>77</v>
       </c>
@@ -4002,11 +4876,22 @@
       <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{wang2} Yue Wang, Quanbao Li, Qinglin Han, Qinghua Ma, Rongbin Ji, Bingwen Song, Wanqi Jie, Yaohe Zhou, Yuko Inatomi. Growth and properties of 40 mm diameter $\mathrm{Hg}_{1-\chi} \mathrm{Cd}_{\mathrm{X}} \mathrm{Te}$ using the two-stage Pressurized Bridgman method. {\itshape Journal of Crystal Growth} 263 (2004) 54-62.</v>
+      </c>
       <c r="G45" s="1" t="s">
         <v>78</v>
       </c>
@@ -4014,15 +4899,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>308</v>
+      </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="F46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">\bibitem{nikiforov} Vladimir Nikiforov (\ru{Никифоров Владимир Николаевиш}), MSU, Private communication. {\itshape } </v>
+      </c>
       <c r="G46" s="1" t="s">
         <v>79</v>
       </c>
@@ -4034,11 +4926,22 @@
       <c r="A47" s="4">
         <v>46</v>
       </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{capper} P. Capper. {\itshape Properties of narrow gap Cadmium-based compounds.} INSPEC, the Institution of Electrical Engineers (1994).</v>
+      </c>
       <c r="G47" s="1" t="s">
         <v>80</v>
       </c>
@@ -4046,15 +4949,26 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>47</v>
       </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{williams} D. J. Williams, A. W. Vere. Sub-grain boundaries in $\mathrm{Cd}_{\mathrm{X}} \mathrm{Hg}_{1-\mathrm{X}} \mathrm{Te}$ and CdTe. {\itshape J. Cryst. Growth} vol. 83 (1987) p. 341-352.</v>
+      </c>
       <c r="G48" s="1" t="s">
         <v>81</v>
       </c>
@@ -4069,10 +4983,19 @@
       <c r="B49" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
+      <c r="C49" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{spicer2} W. E. Spicer, J. A. Silberman, and I. Lindau. Band gap variation and lattice, surface, and interface "instabilities" in $\mathrm{Hg}_{1-\mathrm{x}} \mathrm{Cd}_{\mathrm{x}} \mathrm{Te}$ and related compounds. {\itshape J. Vac. Sci. Technol. A} 1(3) pp. 1735-1743 (1983).</v>
+      </c>
       <c r="G49" s="1" t="s">
         <v>82</v>
       </c>
@@ -4080,15 +5003,26 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>49</v>
       </c>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{morgen} P. Morgen, J. Silberman, I. Landau, W. E. Spicer, J. A. Wilson. Stability of an atomically clean $\mathrm{Hg}_{1-\mathrm{x}} \mathrm{Cd}_{\mathrm{x}} \mathrm{Te}$ surface in vacuum and under $\mathrm{O}_{2}$ exposure. {\itshape Journal of Crystal Growth} 56, 493-497 (1982).</v>
+      </c>
       <c r="G50" s="1" t="s">
         <v>83</v>
       </c>
@@ -4096,15 +5030,22 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>50</v>
       </c>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>341</v>
+      </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+      <c r="F51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">\bibitem{mitdank} R. Mitdank. Mikrosondenanalyse. Beispiele für Untersuchungen an der Elektronenstrahlmikrosonde. \href{http://htc.physik.hu-berlin.de/~mitdank/semq.htm}{http://htc.physik.hu-berlin.de/~mitdank/semq.htm}. {\itshape } </v>
+      </c>
       <c r="G51" s="1" t="s">
         <v>84</v>
       </c>
@@ -4112,15 +5053,26 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>51</v>
       </c>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
+      <c r="B52" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{berding} M. A. Berding, A. Sher, A-B Chen and R. Patrick. Vacancies and surface segregation in HgCdTe and HgZnTe. {\itshape Semicond. Sci. Technol.} vol.  {\bfseries 5} pp. S86-S89 (1990).</v>
+      </c>
       <c r="G52" s="1" t="s">
         <v>85</v>
       </c>
@@ -4128,15 +5080,26 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>52</v>
       </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{ribbat} C. Ribbat. Aufbau einer MBE-Anlage zur Herstellung von MolybdändichalkogenidSchichtkristallen für photovoltaische Anwendungen. {\itshape Diplomarbeit,} AG EES, (1998).</v>
+      </c>
       <c r="G53" s="1" t="s">
         <v>86</v>
       </c>
@@ -4148,11 +5111,22 @@
       <c r="A54" s="4">
         <v>53</v>
       </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{silberman} J. A. Silberman, P. Morgen, I. Lindau, and W. E. Spicer. UPS study of the electronic structure of $\mathrm{Hg_{1-X}Cd_XTe}$: Breakdown of the virtual crystal approximation. {\itshape J. Vac. Sci. Technol.} 21(1) pp. 142-145 (1982).</v>
+      </c>
       <c r="G54" s="1" t="s">
         <v>87</v>
       </c>
@@ -4160,15 +5134,26 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>54</v>
       </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
+      <c r="B55" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{shih} C. K. Shih and W. E. Spicer. Photoemission studies of core level shifts in $\mathrm{HgCdTe}, \mathrm{CdMnTe}$, and HgZnTe. {\itshape J. Vac. Sci. Technol. A,} 5(5) pp. 3031-3034 (1987).</v>
+      </c>
       <c r="G55" s="1" t="s">
         <v>88</v>
       </c>
@@ -4180,29 +5165,45 @@
       <c r="A56" s="4">
         <v>55</v>
       </c>
-      <c r="B56" s="1"/>
+      <c r="B56" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="C56" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
+        <v>345</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{shih2} C. K. Shih, J. A. Silberman, A. K. Wahi, G. P. Carey, I. Lindau, and W. E. Spicer. Angle resolved photoemission study of the alloy scattering effect in $\mathrm{Hg_{1-X}Cd_XTe}$. {\itshape  J. Vac. Sci. Technol. A,} 5(5) pp. 3026-3030 (1987).</v>
+      </c>
       <c r="G56" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>56</v>
       </c>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
+      <c r="B57" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>277</v>
+      </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
+      <c r="F57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">\bibitem{puettner} Dr. Ralph Püttner, FU Berlin. Beamlinebetreuer BUS. Private communication. {\itshape } </v>
+      </c>
       <c r="G57" s="1" t="s">
         <v>89</v>
       </c>
@@ -4210,17 +5211,28 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>57</v>
       </c>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
+      <c r="B58" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{moon} Chang-Youn Moon, Su-Huai Wei. Band gap of Hg chalcogenides: Symmetry-reduction-induced band-gap opening of materials with inverted band structures. {\itshape Phys. Rev.} {\bfseries B} 74:045205 (2006).</v>
+      </c>
       <c r="G58" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>56</v>
@@ -4230,29 +5242,51 @@
       <c r="A59" s="4">
         <v>58</v>
       </c>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
+      <c r="B59" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{moulder} J. F. Moulder, W. F. Stickle, P. E. Sobol, K. D. Bomben. {\itshape Handbook of X-ray Photoelectron Spectroscopy.} Perkin-Elmer Corporation, 1992.</v>
+      </c>
       <c r="G59" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>59</v>
       </c>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
+      <c r="B60" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{janowitz2} C. Janowitz, N. Orlowski, R. Manzke, Z. Golacki. On the band structure of HgTe and HgSe - view from photoemission. {\itshape Journal of Alloys and Compounds,} 328, 84-89, (2001).</v>
+      </c>
       <c r="G60" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>58</v>
@@ -4262,51 +5296,78 @@
       <c r="A61" s="4">
         <v>60</v>
       </c>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
+      <c r="B61" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F61" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{fleszar} A. Fleszar, W. Hanke. Electronic structure of $\mathrm{II}^{\mathrm{B}}$-VI semiconductors in the GW approximation. {\itshape Phys. Rev.} {\bfseries B} 71:045207 (2005).</v>
+      </c>
       <c r="G61" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>61</v>
       </c>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
+      <c r="B62" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="F62" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{chen} A-B Chen, Y-M Lai-Hsu, S. Krishnamurthy, M. A. Berding, and A. Sher. Band structures of HgCdTe and HgZnTe alloys and superlattices. {\itshape Semicond. Sci. Technol.} vol. {\bfseries 5} pp. S100-S102 (1990). doi:\href{http://dx.doi.org/10.1088/0268-1242/5/3S/021}{10.1088/0268-1242/5/3S/021}</v>
+      </c>
       <c r="G62" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>62</v>
       </c>
-      <c r="B63" s="1"/>
+      <c r="B63" s="1" t="s">
+        <v>287</v>
+      </c>
       <c r="C63" s="1" t="s">
-        <v>94</v>
+        <v>312</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F63" s="1"/>
+        <v>289</v>
+      </c>
+      <c r="F63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{kane} E. O. Kane. Band structure of indium antimonide. {\itshape J. Phys. Chem. Solids} 1 (4), 249-261 (1957)</v>
+      </c>
       <c r="G63" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>61</v>
@@ -4316,17 +5377,22 @@
       <c r="A64" s="4">
         <v>63</v>
       </c>
-      <c r="B64" s="1"/>
+      <c r="B64" s="1" t="s">
+        <v>288</v>
+      </c>
       <c r="C64" s="1" t="s">
-        <v>91</v>
+        <v>343</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>92</v>
+        <v>321</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F64" s="1"/>
+        <v>290</v>
+      </c>
+      <c r="F64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>\bibitem{janowitz3} C. Janowitz, L. Kipp, R. Manzke. Experimental surface band structure of CdTe(110). {\itshape Surface Science} 231 (1990) 25-31.</v>
+      </c>
       <c r="G64" s="1" t="s">
         <v>90</v>
       </c>

</xml_diff>